<commit_message>
v5 and v6 uploaded
</commit_message>
<xml_diff>
--- a/SoftPACTesting/bin/resources/data/DDT.xlsx
+++ b/SoftPACTesting/bin/resources/data/DDT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F413C8D-D804-4575-9134-7128B69D7C2E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5EFC37B5-AF05-405C-9B68-6CA72D9BB301}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -124,7 +124,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -408,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,10 +436,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -455,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514BFD99-4204-4030-86CA-47FBED926B7C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>